<commit_message>
edit database table. adjust for yuko-tab, yuko-carousel, yuko-img-card
</commit_message>
<xml_diff>
--- a/DataBase/database-design.xlsx
+++ b/DataBase/database-design.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R_Article" sheetId="1" r:id="rId1"/>
-    <sheet name="Table - R_User" sheetId="2" r:id="rId2"/>
-    <sheet name="Table - R_Admin" sheetId="3" r:id="rId3"/>
+    <sheet name="Table - R_Comment" sheetId="6" r:id="rId2"/>
+    <sheet name="Table - R_User" sheetId="2" r:id="rId3"/>
+    <sheet name="Table - R_Admin" sheetId="3" r:id="rId4"/>
+    <sheet name="Table - R_NavBar" sheetId="4" r:id="rId5"/>
+    <sheet name="Table - R_SideBar" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="130">
   <si>
     <t>id</t>
   </si>
@@ -364,14 +367,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1 &gt; female, 2 &gt; male</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-1 &gt; not auth,0 &gt; normal, 1 &gt; limited, 2 &gt; banned</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>readCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -384,13 +379,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>Comment of article</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Table - R_User</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -428,6 +416,126 @@
   </si>
   <si>
     <t>Key for calculating two-step verification code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table - R_NavBar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 &gt; invalid, 1 &gt; valid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parentID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level of this item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Show name of this item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index of this item (Order by)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parent id of this item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Null represented as first level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table - R_SideBar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-3 &gt; not auth,1 &gt; normal, -2 &gt; limited, -3 &gt; banned</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 &gt; female, 2 &gt; male, 0 &gt; UNKNOWN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table - R_Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User ID whose create thi comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Content of this comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create time of this comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteDown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This comment is useful or recomment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This comment is not useful or no recomment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>replyFor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Null represented as a nomal comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If this is a reply for comment, restore its id here</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>articleID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The article's ID that is commented</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -834,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1082,55 +1190,41 @@
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="3"/>
+      <c r="A17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1144,10 +1238,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="39.625" customWidth="1"/>
+    <col min="6" max="6" width="46.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1449,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1284,12 +1571,14 @@
       <c r="C8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1392,12 +1681,14 @@
       <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
       <c r="E15" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1410,12 +1701,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1429,7 +1720,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1495,7 +1786,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>86</v>
@@ -1505,7 +1796,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -1537,7 +1828,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1553,23 +1844,21 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -1583,12 +1872,14 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1599,4 +1890,327 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.875" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="17.75" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
+    <col min="6" max="6" width="66" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="19.875" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
+    <col min="6" max="6" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cms login, including verification and two-step verification
</commit_message>
<xml_diff>
--- a/DataBase/database-design.xlsx
+++ b/DataBase/database-design.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="735" activeTab="3"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="138">
   <si>
     <t>id</t>
   </si>
@@ -307,14 +307,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>thumb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thumb of article</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>datetime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -536,6 +528,46 @@
   </si>
   <si>
     <t>The article's ID that is commented</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cover of article</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addLicense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Additional license of article</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDraft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is this article a draft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Using changeable key to encrypt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -942,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -993,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -1100,131 +1132,161 @@
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3">
         <v>0</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="E18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1256,7 +1318,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1304,7 +1366,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -1314,13 +1376,13 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>37</v>
@@ -1330,7 +1392,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -1346,7 +1408,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>24</v>
@@ -1357,20 +1419,20 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>37</v>
@@ -1378,15 +1440,15 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>37</v>
@@ -1398,13 +1460,13 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>37</v>
@@ -1416,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -1449,7 +1511,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1497,13 +1559,13 @@
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
@@ -1513,7 +1575,7 @@
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>35</v>
@@ -1532,7 +1594,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>2</v>
@@ -1547,7 +1609,7 @@
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>20</v>
@@ -1569,7 +1631,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1578,12 +1640,12 @@
         <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>53</v>
@@ -1597,7 +1659,7 @@
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>20</v>
@@ -1611,7 +1673,7 @@
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>22</v>
@@ -1625,7 +1687,7 @@
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>49</v>
@@ -1641,7 +1703,7 @@
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>49</v>
@@ -1673,7 +1735,7 @@
     </row>
     <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>38</v>
@@ -1688,7 +1750,7 @@
         <v>48</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1706,7 +1768,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1720,7 +1782,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1771,7 +1833,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1781,28 +1843,28 @@
         <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>20</v>
@@ -1818,7 +1880,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
@@ -1828,7 +1890,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1844,27 +1906,27 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>37</v>
@@ -1876,10 +1938,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1912,7 +1974,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1960,23 +2022,23 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -1988,13 +2050,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2006,13 +2068,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -2020,15 +2082,15 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>37</v>
@@ -2040,10 +2102,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2076,7 +2138,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2124,23 +2186,23 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -2150,13 +2212,13 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2168,13 +2230,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -2182,15 +2244,15 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>37</v>
@@ -2200,10 +2262,10 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add db table param - Article.categorys. optimization for cms index, including article management module
</commit_message>
<xml_diff>
--- a/DataBase/database-design.xlsx
+++ b/DataBase/database-design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="735"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R_Article" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="140">
   <si>
     <t>id</t>
   </si>
@@ -568,6 +568,14 @@
   </si>
   <si>
     <t>Using changeable key to encrypt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>categorys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category of article</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -974,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1192,7 +1200,7 @@
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>17</v>
@@ -1200,93 +1208,107 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3">
         <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1767,7 +1789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adjust for some components. Some bugs fixed also.
</commit_message>
<xml_diff>
--- a/DataBase/database-design.xlsx
+++ b/DataBase/database-design.xlsx
@@ -4,15 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="735" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R_Article" sheetId="1" r:id="rId1"/>
     <sheet name="Table - R_Comment" sheetId="6" r:id="rId2"/>
     <sheet name="Table - R_User" sheetId="2" r:id="rId3"/>
     <sheet name="Table - R_Admin" sheetId="3" r:id="rId4"/>
-    <sheet name="Table - R_NavBar" sheetId="4" r:id="rId5"/>
-    <sheet name="Table - R_SideBar" sheetId="5" r:id="rId6"/>
+    <sheet name="Table - R_Role" sheetId="7" r:id="rId5"/>
+    <sheet name="Table - R_Module" sheetId="8" r:id="rId6"/>
+    <sheet name="Table - R_RolePriv" sheetId="9" r:id="rId7"/>
+    <sheet name="Table - R_NavBar" sheetId="4" r:id="rId8"/>
+    <sheet name="Table - R_SideBar" sheetId="5" r:id="rId9"/>
+    <sheet name="Table - R_BlockIP" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="185">
   <si>
     <t>id</t>
   </si>
@@ -379,10 +383,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Authority of Admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Admin's lastest login time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -399,10 +399,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>authority</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -576,6 +572,194 @@
   </si>
   <si>
     <t>Category of article</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table - R_Role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name of Role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code of Role, including ROOT/ADMINISTRATOR/NORMAL/GUEST etc.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> ROOT-Super administrator/ADMINISTRATOR-Administrator/NORMAL-Normal user/GUEST-Guest user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Role of Admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table - R_Module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT NULL </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is this role enabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is this module enabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name of module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Specific code of module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table - R_RolePriv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roleID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID of role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moduleID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID of module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is this priv of role vaild</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roleID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tryCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 &gt; blocked, 1 &gt; allow access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP adrdress try times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last try time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table - R_BlockIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastTryTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP adrdress try times(two-step verification)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tryCountTsv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -625,7 +809,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -672,11 +856,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -699,6 +896,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -984,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -999,14 +1200,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1033,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -1140,15 +1341,15 @@
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="7"/>
       <c r="E10" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -1200,7 +1401,7 @@
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>17</v>
@@ -1208,7 +1409,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -1274,23 +1475,23 @@
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3">
         <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>22</v>
@@ -1298,7 +1499,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" s="5"/>
     </row>
@@ -1309,6 +1510,168 @@
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="35.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1339,14 +1702,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1388,7 +1751,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -1398,13 +1761,13 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>37</v>
@@ -1414,7 +1777,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -1430,7 +1793,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>24</v>
@@ -1441,20 +1804,20 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>37</v>
@@ -1462,15 +1825,15 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>37</v>
@@ -1482,13 +1845,13 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>37</v>
@@ -1500,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -1518,7 +1881,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F15" sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1532,14 +1895,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1662,7 +2025,7 @@
         <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1772,7 +2135,7 @@
         <v>48</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1790,7 +2153,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1803,14 +2166,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1865,12 +2228,12 @@
         <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>84</v>
@@ -1880,7 +2243,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -1912,7 +2275,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1928,21 +2291,23 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -1960,10 +2325,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1977,6 +2342,389 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="40.625" customWidth="1"/>
+    <col min="6" max="6" width="44.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="55.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
+    <col min="6" max="6" width="45.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1995,14 +2743,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2044,23 +2792,23 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -2072,13 +2820,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2090,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -2104,10 +2852,10 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2124,10 +2872,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2140,12 +2888,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2159,14 +2907,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2208,23 +2956,23 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -2234,13 +2982,13 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2252,13 +3000,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -2266,10 +3014,10 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2284,10 +3032,10 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>